<commit_message>
The rapport has been updated with an adjusted GANTT and removed non participating team members from the econmic calulations
</commit_message>
<xml_diff>
--- a/doc/rapport/detaljerad-planering.xlsx
+++ b/doc/rapport/detaljerad-planering.xlsx
@@ -140,7 +140,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,12 +222,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,22 +398,20 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -433,24 +425,26 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -804,7 +798,7 @@
   <dimension ref="A1:AL19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -815,99 +809,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="19" customHeight="1">
-      <c r="B1" s="53">
+      <c r="B1" s="54">
         <v>40506</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54">
         <v>40507</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53">
+      <c r="E1" s="54"/>
+      <c r="F1" s="54">
         <v>40508</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="56" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="53">
+      <c r="I1" s="54">
         <v>40511</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53">
+      <c r="J1" s="54"/>
+      <c r="K1" s="54">
         <v>40512</v>
       </c>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53">
+      <c r="L1" s="54"/>
+      <c r="M1" s="54">
         <v>40513</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53">
+      <c r="N1" s="54"/>
+      <c r="O1" s="54">
         <v>40514</v>
       </c>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53">
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54">
         <v>40515</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="56" t="s">
+      <c r="R1" s="54"/>
+      <c r="S1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="53">
+      <c r="T1" s="54">
         <v>40518</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53">
+      <c r="U1" s="54"/>
+      <c r="V1" s="54">
         <v>40519</v>
       </c>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53">
+      <c r="W1" s="54"/>
+      <c r="X1" s="54">
         <v>40520</v>
       </c>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53">
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54">
         <v>40521</v>
       </c>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53">
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54">
         <v>40522</v>
       </c>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="56" t="s">
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" s="53">
+      <c r="AE1" s="54">
         <v>40525</v>
       </c>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53">
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54">
         <v>40526</v>
       </c>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53">
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54">
         <v>40527</v>
       </c>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53">
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54">
         <v>40528</v>
       </c>
-      <c r="AL1" s="53"/>
+      <c r="AL1" s="54"/>
     </row>
     <row r="2" spans="1:38" ht="23" customHeight="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="42"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
       <c r="M2" s="2"/>
       <c r="N2" s="3"/>
       <c r="O2" s="2"/>
@@ -921,22 +915,22 @@
       <c r="W2" s="3"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="3"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="46"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="44"/>
       <c r="AD2" s="4"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="46"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="45"/>
-      <c r="AL2" s="46"/>
+      <c r="AE2" s="43"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="43"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="43"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="43"/>
+      <c r="AL2" s="44"/>
     </row>
     <row r="3" spans="1:38" ht="23" customHeight="1">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="48" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2"/>
@@ -946,10 +940,10 @@
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="44"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="42"/>
       <c r="M3" s="2"/>
       <c r="N3" s="3"/>
       <c r="O3" s="2"/>
@@ -963,22 +957,22 @@
       <c r="W3" s="3"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="3"/>
-      <c r="Z3" s="47"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="47"/>
-      <c r="AC3" s="48"/>
+      <c r="Z3" s="45"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="45"/>
+      <c r="AC3" s="46"/>
       <c r="AD3" s="4"/>
-      <c r="AE3" s="47"/>
-      <c r="AF3" s="48"/>
-      <c r="AG3" s="47"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="47"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="47"/>
-      <c r="AL3" s="48"/>
+      <c r="AE3" s="45"/>
+      <c r="AF3" s="46"/>
+      <c r="AG3" s="45"/>
+      <c r="AH3" s="46"/>
+      <c r="AI3" s="45"/>
+      <c r="AJ3" s="46"/>
+      <c r="AK3" s="45"/>
+      <c r="AL3" s="46"/>
     </row>
     <row r="4" spans="1:38" ht="23" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="49" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="2"/>
@@ -992,9 +986,9 @@
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="26"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="24"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="3"/>
@@ -1005,22 +999,22 @@
       <c r="W4" s="3"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="3"/>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="48"/>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="48"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="46"/>
+      <c r="AB4" s="45"/>
+      <c r="AC4" s="46"/>
       <c r="AD4" s="4"/>
-      <c r="AE4" s="47"/>
-      <c r="AF4" s="48"/>
-      <c r="AG4" s="47"/>
-      <c r="AH4" s="48"/>
-      <c r="AI4" s="47"/>
-      <c r="AJ4" s="48"/>
-      <c r="AK4" s="47"/>
-      <c r="AL4" s="48"/>
+      <c r="AE4" s="45"/>
+      <c r="AF4" s="46"/>
+      <c r="AG4" s="45"/>
+      <c r="AH4" s="46"/>
+      <c r="AI4" s="45"/>
+      <c r="AJ4" s="46"/>
+      <c r="AK4" s="45"/>
+      <c r="AL4" s="46"/>
     </row>
     <row r="5" spans="1:38" ht="23" customHeight="1">
-      <c r="A5" s="52"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
@@ -1045,22 +1039,22 @@
       <c r="W5" s="3"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="3"/>
-      <c r="Z5" s="47"/>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="48"/>
+      <c r="Z5" s="45"/>
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="46"/>
       <c r="AD5" s="4"/>
-      <c r="AE5" s="47"/>
-      <c r="AF5" s="48"/>
-      <c r="AG5" s="47"/>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="47"/>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="47"/>
-      <c r="AL5" s="48"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="45"/>
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="45"/>
+      <c r="AL5" s="46"/>
     </row>
     <row r="6" spans="1:38" ht="23" customHeight="1">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="2"/>
@@ -1077,9 +1071,9 @@
       <c r="M6" s="2"/>
       <c r="N6" s="3"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="28"/>
+      <c r="P6" s="26"/>
       <c r="Q6" s="5"/>
-      <c r="R6" s="28"/>
+      <c r="R6" s="26"/>
       <c r="S6" s="4"/>
       <c r="T6" s="2"/>
       <c r="U6" s="3"/>
@@ -1087,22 +1081,22 @@
       <c r="W6" s="3"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="3"/>
-      <c r="Z6" s="47"/>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="47"/>
-      <c r="AC6" s="48"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="46"/>
+      <c r="AB6" s="45"/>
+      <c r="AC6" s="46"/>
       <c r="AD6" s="4"/>
-      <c r="AE6" s="47"/>
-      <c r="AF6" s="48"/>
-      <c r="AG6" s="47"/>
-      <c r="AH6" s="48"/>
-      <c r="AI6" s="47"/>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="47"/>
-      <c r="AL6" s="48"/>
+      <c r="AE6" s="45"/>
+      <c r="AF6" s="46"/>
+      <c r="AG6" s="45"/>
+      <c r="AH6" s="46"/>
+      <c r="AI6" s="45"/>
+      <c r="AJ6" s="46"/>
+      <c r="AK6" s="45"/>
+      <c r="AL6" s="46"/>
     </row>
     <row r="7" spans="1:38" ht="23" customHeight="1">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2"/>
@@ -1144,7 +1138,7 @@
       <c r="AL7" s="3"/>
     </row>
     <row r="8" spans="1:38" ht="23" customHeight="1">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="2"/>
@@ -1186,7 +1180,7 @@
       <c r="AL8" s="3"/>
     </row>
     <row r="9" spans="1:38" ht="23" customHeight="1">
-      <c r="A9" s="32"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
@@ -1226,7 +1220,7 @@
       <c r="AL9" s="3"/>
     </row>
     <row r="10" spans="1:38" ht="23" customHeight="1">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="31" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2"/>
@@ -1260,15 +1254,15 @@
       <c r="AD10" s="4"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="3"/>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="2"/>
-      <c r="AJ10" s="3"/>
+      <c r="AG10" s="16"/>
+      <c r="AH10" s="17"/>
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="11"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="3"/>
     </row>
     <row r="11" spans="1:38" ht="23" customHeight="1">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2"/>
@@ -1291,26 +1285,26 @@
       <c r="S11" s="4"/>
       <c r="T11" s="2"/>
       <c r="U11" s="3"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="13"/>
+      <c r="V11" s="55"/>
+      <c r="W11" s="56"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="12"/>
-      <c r="AC11" s="13"/>
+      <c r="Z11" s="55"/>
+      <c r="AA11" s="56"/>
+      <c r="AB11" s="55"/>
+      <c r="AC11" s="56"/>
       <c r="AD11" s="4"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="3"/>
       <c r="AG11" s="2"/>
-      <c r="AH11" s="13"/>
-      <c r="AI11" s="12"/>
-      <c r="AJ11" s="13"/>
+      <c r="AH11" s="56"/>
+      <c r="AI11" s="55"/>
+      <c r="AJ11" s="56"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="3"/>
     </row>
     <row r="12" spans="1:38" ht="23" customHeight="1">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2"/>
@@ -1333,14 +1327,14 @@
       <c r="S12" s="4"/>
       <c r="T12" s="2"/>
       <c r="U12" s="3"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="3"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="13"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="3"/>
@@ -1352,7 +1346,7 @@
       <c r="AL12" s="3"/>
     </row>
     <row r="13" spans="1:38" ht="23" customHeight="1">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2"/>
@@ -1381,20 +1375,20 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="3"/>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="17"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="15"/>
       <c r="AD13" s="4"/>
-      <c r="AE13" s="16"/>
-      <c r="AF13" s="17"/>
-      <c r="AG13" s="18"/>
-      <c r="AH13" s="19"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="16"/>
+      <c r="AH13" s="17"/>
       <c r="AI13" s="2"/>
       <c r="AJ13" s="3"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="3"/>
     </row>
     <row r="14" spans="1:38" ht="23" customHeight="1">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="2"/>
@@ -1426,17 +1420,17 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="4"/>
-      <c r="AE14" s="54"/>
-      <c r="AF14" s="55"/>
-      <c r="AG14" s="54"/>
-      <c r="AH14" s="55"/>
-      <c r="AI14" s="54"/>
+      <c r="AE14" s="51"/>
+      <c r="AF14" s="52"/>
+      <c r="AG14" s="51"/>
+      <c r="AH14" s="52"/>
+      <c r="AI14" s="51"/>
       <c r="AJ14" s="3"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="3"/>
     </row>
     <row r="15" spans="1:38" ht="23" customHeight="1">
-      <c r="A15" s="32"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
@@ -1476,7 +1470,7 @@
       <c r="AL15" s="3"/>
     </row>
     <row r="16" spans="1:38" ht="23" customHeight="1">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2"/>
@@ -1508,17 +1502,17 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="4"/>
-      <c r="AE16" s="20"/>
-      <c r="AF16" s="21"/>
-      <c r="AG16" s="20"/>
-      <c r="AH16" s="21"/>
-      <c r="AI16" s="20"/>
-      <c r="AJ16" s="19"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="19"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="19"/>
+      <c r="AI16" s="18"/>
+      <c r="AJ16" s="17"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="3"/>
     </row>
     <row r="17" spans="1:38" ht="23" customHeight="1">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2"/>
@@ -1553,14 +1547,14 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="2"/>
-      <c r="AH17" s="25"/>
-      <c r="AI17" s="24"/>
-      <c r="AJ17" s="25"/>
+      <c r="AH17" s="23"/>
+      <c r="AI17" s="22"/>
+      <c r="AJ17" s="23"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="3"/>
     </row>
     <row r="18" spans="1:38" ht="23" customHeight="1">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="2"/>
@@ -1596,14 +1590,19 @@
       <c r="AF18" s="3"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="3"/>
-      <c r="AI18" s="22"/>
-      <c r="AJ18" s="23"/>
-      <c r="AK18" s="22"/>
-      <c r="AL18" s="23"/>
+      <c r="AI18" s="20"/>
+      <c r="AJ18" s="21"/>
+      <c r="AK18" s="20"/>
+      <c r="AL18" s="21"/>
     </row>
     <row r="19" spans="1:38" ht="23" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="AK1:AL1"/>
@@ -1616,15 +1615,9 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="65" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="24" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>